<commit_message>
, per i casi di test con ID [35, 43, 51], riportato in colonna “Messaggio di errore”, l’errore visualizzato a video dall’utente, e in colonna “Gestione errore”, le modalità di gestione dell’errore
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111ELCO0000000/asl2savonese/onesys-ps/2.6.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111ELCO0000000/asl2savonese/onesys-ps/2.6.0/report-checklist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luca.martinelli\OneDrive - EL.CO. - S.R.L\Desktop\FSE 2.0\Accreditamento VPS\DaCertificare\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ACCREDITAMENTO_FSE_ONESYS\GATEWAY\A1#111ELCO0000000\asl2savonese\onesys-ps\2.6.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C878F846-01EA-4D80-BE04-010D873F0B4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4121946F-72F2-4F2D-B0ED-2350727F4F2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Istruzioni Compilazione" sheetId="1" r:id="rId1"/>
@@ -3887,23 +3887,9 @@
     <t>Viene mostrato un messaggio di errore al medico ed è configurabile il fatto di interrompere il processo o permettere al medico di firmare il referto. Il pdf risultante avrà comunque al suo interno il cda2</t>
   </si>
   <si>
-    <t>Il campo purpose_of_use non è valorizzato
-Viene mostrato un messaggio di errore al medico ed è configurabile il fatto di interrompere il processo o permettere al medico di firmare il referto. Il pdf risultante avrà comunque al suo interno il cda2</t>
-  </si>
-  <si>
     <t>SI, Da rivalidare</t>
   </si>
   <si>
-    <t>Rivalidazione in Backoffice</t>
-  </si>
-  <si>
-    <t>Il sistema attende un numero di millisecondi configurabile (default 5000) Dopo tale tempo viene mostrato un messaggio di errore al medico ed è configurabile il fatto di interrompere il processo o permettere al medico di firmare il referto. Il pdf risultante avrà comunque al suo interno il cda2</t>
-  </si>
-  <si>
-    <t>Il campo action_id non è corretto
-Viene mostrato un messaggio di errore al medico ed è configurabile il fatto di interrompere il processo o permettere al medico di firmare il referto. Il pdf risultante avrà comunque al suo interno il cda2</t>
-  </si>
-  <si>
     <t>UNKNOWN_WORKFLOW_ID</t>
   </si>
   <si>
@@ -4145,6 +4131,20 @@
   </si>
   <si>
     <t>2.16.840.1.113883.2.9.2.70102.365997474a39036dad008bfade0c88de56a8d0f94ac5095c5ec684f97a19571c.243f71e950^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Il campo action_id non è corretto
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Il campo purpose_of_use non è valorizzato. 
+</t>
+  </si>
+  <si>
+    <t>Timeout del Gateway</t>
+  </si>
+  <si>
+    <t>In backoffice prima di inviare il referto al repository aziendale viene eseguito un tentativo di reinvio al gateway</t>
   </si>
 </sst>
 </file>
@@ -7076,10 +7076,10 @@
   <dimension ref="A1:T992"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="I327" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="6" topLeftCell="G210" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="K329" sqref="K329"/>
+      <selection pane="bottomRight" activeCell="I226" sqref="I226"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -14049,13 +14049,13 @@
         <v>45097</v>
       </c>
       <c r="G207" s="34" t="s">
-        <v>873</v>
+        <v>869</v>
       </c>
       <c r="H207" s="34" t="s">
-        <v>872</v>
+        <v>868</v>
       </c>
       <c r="I207" s="37" t="s">
-        <v>832</v>
+        <v>828</v>
       </c>
       <c r="J207" s="25" t="s">
         <v>419</v>
@@ -14445,13 +14445,13 @@
         <v>45096</v>
       </c>
       <c r="G218" s="24" t="s">
-        <v>827</v>
+        <v>823</v>
       </c>
       <c r="H218" s="37" t="s">
-        <v>828</v>
+        <v>824</v>
       </c>
       <c r="I218" s="24" t="s">
-        <v>826</v>
+        <v>822</v>
       </c>
       <c r="J218" s="25" t="s">
         <v>419</v>
@@ -14464,13 +14464,13 @@
         <v>419</v>
       </c>
       <c r="N218" s="25" t="s">
+        <v>904</v>
+      </c>
+      <c r="O218" s="25" t="s">
         <v>821</v>
       </c>
-      <c r="O218" s="25" t="s">
-        <v>822</v>
-      </c>
       <c r="P218" s="25" t="s">
-        <v>823</v>
+        <v>906</v>
       </c>
       <c r="Q218" s="25"/>
       <c r="R218" s="26"/>
@@ -14743,13 +14743,13 @@
         <v>45096</v>
       </c>
       <c r="G226" s="24" t="s">
-        <v>829</v>
+        <v>825</v>
       </c>
       <c r="H226" s="34" t="s">
-        <v>830</v>
+        <v>826</v>
       </c>
       <c r="I226" s="24" t="s">
-        <v>826</v>
+        <v>822</v>
       </c>
       <c r="J226" s="25" t="s">
         <v>419</v>
@@ -14762,13 +14762,13 @@
         <v>419</v>
       </c>
       <c r="N226" s="25" t="s">
-        <v>825</v>
+        <v>903</v>
       </c>
       <c r="O226" s="25" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="P226" s="25" t="s">
-        <v>823</v>
+        <v>906</v>
       </c>
       <c r="Q226" s="25"/>
       <c r="R226" s="26"/>
@@ -15049,7 +15049,7 @@
         <v>45096</v>
       </c>
       <c r="G234" s="37" t="s">
-        <v>831</v>
+        <v>827</v>
       </c>
       <c r="H234" s="24"/>
       <c r="I234" s="24"/>
@@ -15064,13 +15064,13 @@
         <v>419</v>
       </c>
       <c r="N234" s="25" t="s">
-        <v>824</v>
+        <v>905</v>
       </c>
       <c r="O234" s="25" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="P234" s="25" t="s">
-        <v>823</v>
+        <v>906</v>
       </c>
       <c r="Q234" s="25"/>
       <c r="R234" s="26" t="s">
@@ -17481,13 +17481,13 @@
         <v>45096</v>
       </c>
       <c r="G305" s="24" t="s">
-        <v>837</v>
+        <v>833</v>
       </c>
       <c r="H305" s="24" t="s">
-        <v>836</v>
+        <v>832</v>
       </c>
       <c r="I305" s="24" t="s">
-        <v>833</v>
+        <v>829</v>
       </c>
       <c r="J305" s="35" t="s">
         <v>419</v>
@@ -17500,13 +17500,13 @@
         <v>419</v>
       </c>
       <c r="N305" s="25" t="s">
-        <v>834</v>
+        <v>830</v>
       </c>
       <c r="O305" s="35" t="s">
         <v>419</v>
       </c>
       <c r="P305" s="35" t="s">
-        <v>835</v>
+        <v>831</v>
       </c>
       <c r="Q305" s="25"/>
       <c r="R305" s="26"/>
@@ -17535,13 +17535,13 @@
         <v>45096</v>
       </c>
       <c r="G306" s="24" t="s">
-        <v>838</v>
+        <v>834</v>
       </c>
       <c r="H306" s="24" t="s">
-        <v>839</v>
+        <v>835</v>
       </c>
       <c r="I306" s="37" t="s">
-        <v>833</v>
+        <v>829</v>
       </c>
       <c r="J306" s="35" t="s">
         <v>419</v>
@@ -17554,13 +17554,13 @@
         <v>419</v>
       </c>
       <c r="N306" s="25" t="s">
-        <v>840</v>
+        <v>836</v>
       </c>
       <c r="O306" s="25" t="s">
         <v>419</v>
       </c>
       <c r="P306" s="35" t="s">
-        <v>835</v>
+        <v>831</v>
       </c>
       <c r="Q306" s="25"/>
       <c r="R306" s="26"/>
@@ -17589,13 +17589,13 @@
         <v>45096</v>
       </c>
       <c r="G307" s="24" t="s">
-        <v>841</v>
+        <v>837</v>
       </c>
       <c r="H307" s="24" t="s">
-        <v>842</v>
+        <v>838</v>
       </c>
       <c r="I307" s="24" t="s">
-        <v>843</v>
+        <v>839</v>
       </c>
       <c r="J307" s="35" t="s">
         <v>419</v>
@@ -17608,13 +17608,13 @@
         <v>419</v>
       </c>
       <c r="N307" s="25" t="s">
-        <v>844</v>
+        <v>840</v>
       </c>
       <c r="O307" s="25" t="s">
         <v>419</v>
       </c>
       <c r="P307" s="35" t="s">
-        <v>835</v>
+        <v>831</v>
       </c>
       <c r="Q307" s="25"/>
       <c r="R307" s="26"/>
@@ -17643,13 +17643,13 @@
         <v>45096</v>
       </c>
       <c r="G308" s="24" t="s">
-        <v>845</v>
+        <v>841</v>
       </c>
       <c r="H308" s="24" t="s">
-        <v>846</v>
+        <v>842</v>
       </c>
       <c r="I308" s="24" t="s">
-        <v>847</v>
+        <v>843</v>
       </c>
       <c r="J308" s="25" t="s">
         <v>419</v>
@@ -17662,13 +17662,13 @@
         <v>419</v>
       </c>
       <c r="N308" s="25" t="s">
-        <v>848</v>
+        <v>844</v>
       </c>
       <c r="O308" s="25" t="s">
         <v>419</v>
       </c>
       <c r="P308" s="35" t="s">
-        <v>835</v>
+        <v>831</v>
       </c>
       <c r="Q308" s="25"/>
       <c r="R308" s="26"/>
@@ -17697,13 +17697,13 @@
         <v>45096</v>
       </c>
       <c r="G309" s="34" t="s">
-        <v>849</v>
+        <v>845</v>
       </c>
       <c r="H309" s="24" t="s">
-        <v>851</v>
+        <v>847</v>
       </c>
       <c r="I309" s="37" t="s">
-        <v>852</v>
+        <v>848</v>
       </c>
       <c r="J309" s="35" t="s">
         <v>419</v>
@@ -17716,13 +17716,13 @@
         <v>419</v>
       </c>
       <c r="N309" s="25" t="s">
-        <v>850</v>
+        <v>846</v>
       </c>
       <c r="O309" s="25" t="s">
         <v>419</v>
       </c>
       <c r="P309" s="35" t="s">
-        <v>835</v>
+        <v>831</v>
       </c>
       <c r="Q309" s="25"/>
       <c r="R309" s="26"/>
@@ -17751,13 +17751,13 @@
         <v>45096</v>
       </c>
       <c r="G310" s="24" t="s">
-        <v>854</v>
+        <v>850</v>
       </c>
       <c r="H310" s="37" t="s">
-        <v>855</v>
+        <v>851</v>
       </c>
       <c r="I310" s="24" t="s">
-        <v>856</v>
+        <v>852</v>
       </c>
       <c r="J310" s="35" t="s">
         <v>419</v>
@@ -17770,13 +17770,13 @@
         <v>419</v>
       </c>
       <c r="N310" s="35" t="s">
-        <v>853</v>
+        <v>849</v>
       </c>
       <c r="O310" s="25" t="s">
         <v>419</v>
       </c>
       <c r="P310" s="35" t="s">
-        <v>835</v>
+        <v>831</v>
       </c>
       <c r="Q310" s="25"/>
       <c r="R310" s="26"/>
@@ -17805,13 +17805,13 @@
         <v>45096</v>
       </c>
       <c r="G311" s="24" t="s">
-        <v>857</v>
+        <v>853</v>
       </c>
       <c r="H311" s="24" t="s">
-        <v>858</v>
+        <v>854</v>
       </c>
       <c r="I311" s="24" t="s">
-        <v>859</v>
+        <v>855</v>
       </c>
       <c r="J311" s="25" t="s">
         <v>419</v>
@@ -17824,13 +17824,13 @@
         <v>419</v>
       </c>
       <c r="N311" s="25" t="s">
-        <v>860</v>
+        <v>856</v>
       </c>
       <c r="O311" s="25" t="s">
         <v>419</v>
       </c>
       <c r="P311" s="35" t="s">
-        <v>835</v>
+        <v>831</v>
       </c>
       <c r="Q311" s="25"/>
       <c r="R311" s="26"/>
@@ -17859,13 +17859,13 @@
         <v>45097</v>
       </c>
       <c r="G312" s="24" t="s">
-        <v>861</v>
+        <v>857</v>
       </c>
       <c r="H312" s="24" t="s">
-        <v>862</v>
+        <v>858</v>
       </c>
       <c r="I312" s="24" t="s">
-        <v>863</v>
+        <v>859</v>
       </c>
       <c r="J312" s="25" t="s">
         <v>419</v>
@@ -17878,13 +17878,13 @@
         <v>419</v>
       </c>
       <c r="N312" s="41" t="s">
-        <v>864</v>
+        <v>860</v>
       </c>
       <c r="O312" s="25" t="s">
         <v>419</v>
       </c>
       <c r="P312" s="35" t="s">
-        <v>835</v>
+        <v>831</v>
       </c>
       <c r="Q312" s="25"/>
       <c r="R312" s="26"/>
@@ -17913,13 +17913,13 @@
         <v>45097</v>
       </c>
       <c r="G313" s="24" t="s">
-        <v>865</v>
+        <v>861</v>
       </c>
       <c r="H313" s="24" t="s">
-        <v>866</v>
+        <v>862</v>
       </c>
       <c r="I313" s="24" t="s">
-        <v>867</v>
+        <v>863</v>
       </c>
       <c r="J313" s="25" t="s">
         <v>419</v>
@@ -17932,13 +17932,13 @@
         <v>419</v>
       </c>
       <c r="N313" s="35" t="s">
-        <v>868</v>
+        <v>864</v>
       </c>
       <c r="O313" s="25" t="s">
         <v>419</v>
       </c>
       <c r="P313" s="35" t="s">
-        <v>835</v>
+        <v>831</v>
       </c>
       <c r="Q313" s="25"/>
       <c r="R313" s="26"/>
@@ -17967,13 +17967,13 @@
         <v>45097</v>
       </c>
       <c r="G314" s="24" t="s">
-        <v>869</v>
+        <v>865</v>
       </c>
       <c r="H314" s="24" t="s">
-        <v>870</v>
+        <v>866</v>
       </c>
       <c r="I314" s="24" t="s">
-        <v>871</v>
+        <v>867</v>
       </c>
       <c r="J314" s="25" t="s">
         <v>419</v>
@@ -17986,13 +17986,13 @@
         <v>419</v>
       </c>
       <c r="N314" s="25" t="s">
-        <v>875</v>
+        <v>871</v>
       </c>
       <c r="O314" s="25" t="s">
         <v>419</v>
       </c>
       <c r="P314" s="35" t="s">
-        <v>835</v>
+        <v>831</v>
       </c>
       <c r="Q314" s="25"/>
       <c r="R314" s="26"/>
@@ -18021,13 +18021,13 @@
         <v>45097</v>
       </c>
       <c r="G315" s="24" t="s">
-        <v>876</v>
+        <v>872</v>
       </c>
       <c r="H315" s="24" t="s">
-        <v>877</v>
+        <v>873</v>
       </c>
       <c r="I315" s="24" t="s">
-        <v>878</v>
+        <v>874</v>
       </c>
       <c r="J315" s="25" t="s">
         <v>419</v>
@@ -18040,13 +18040,13 @@
         <v>419</v>
       </c>
       <c r="N315" s="25" t="s">
-        <v>874</v>
+        <v>870</v>
       </c>
       <c r="O315" s="25" t="s">
         <v>419</v>
       </c>
       <c r="P315" s="35" t="s">
-        <v>835</v>
+        <v>831</v>
       </c>
       <c r="Q315" s="25"/>
       <c r="R315" s="26"/>
@@ -18075,13 +18075,13 @@
         <v>45097</v>
       </c>
       <c r="G316" s="24" t="s">
-        <v>882</v>
+        <v>878</v>
       </c>
       <c r="H316" s="24" t="s">
-        <v>880</v>
+        <v>876</v>
       </c>
       <c r="I316" s="24" t="s">
-        <v>881</v>
+        <v>877</v>
       </c>
       <c r="J316" s="25" t="s">
         <v>419</v>
@@ -18094,13 +18094,13 @@
         <v>419</v>
       </c>
       <c r="N316" s="25" t="s">
-        <v>879</v>
+        <v>875</v>
       </c>
       <c r="O316" s="25" t="s">
         <v>419</v>
       </c>
       <c r="P316" s="35" t="s">
-        <v>835</v>
+        <v>831</v>
       </c>
       <c r="Q316" s="25"/>
       <c r="R316" s="26"/>
@@ -18133,7 +18133,7 @@
         <v>422</v>
       </c>
       <c r="K317" s="35" t="s">
-        <v>883</v>
+        <v>879</v>
       </c>
       <c r="L317" s="35"/>
       <c r="M317" s="35"/>
@@ -18171,7 +18171,7 @@
         <v>422</v>
       </c>
       <c r="K318" s="35" t="s">
-        <v>883</v>
+        <v>879</v>
       </c>
       <c r="L318" s="35"/>
       <c r="M318" s="35"/>
@@ -18209,7 +18209,7 @@
         <v>422</v>
       </c>
       <c r="K319" s="35" t="s">
-        <v>883</v>
+        <v>879</v>
       </c>
       <c r="L319" s="35"/>
       <c r="M319" s="35"/>
@@ -18247,7 +18247,7 @@
         <v>422</v>
       </c>
       <c r="K320" s="35" t="s">
-        <v>884</v>
+        <v>880</v>
       </c>
       <c r="L320" s="35"/>
       <c r="M320" s="35"/>
@@ -18285,7 +18285,7 @@
         <v>422</v>
       </c>
       <c r="K321" s="35" t="s">
-        <v>885</v>
+        <v>881</v>
       </c>
       <c r="L321" s="35"/>
       <c r="M321" s="35"/>
@@ -18319,13 +18319,13 @@
         <v>45097</v>
       </c>
       <c r="G322" s="24" t="s">
-        <v>887</v>
+        <v>883</v>
       </c>
       <c r="H322" s="24" t="s">
-        <v>889</v>
+        <v>885</v>
       </c>
       <c r="I322" s="24" t="s">
-        <v>890</v>
+        <v>886</v>
       </c>
       <c r="J322" s="41" t="s">
         <v>419</v>
@@ -18338,13 +18338,13 @@
         <v>419</v>
       </c>
       <c r="N322" s="25" t="s">
-        <v>886</v>
+        <v>882</v>
       </c>
       <c r="O322" s="25" t="s">
         <v>419</v>
       </c>
       <c r="P322" s="35" t="s">
-        <v>835</v>
+        <v>831</v>
       </c>
       <c r="Q322" s="25"/>
       <c r="R322" s="26"/>
@@ -18373,13 +18373,13 @@
         <v>45097</v>
       </c>
       <c r="G323" s="24" t="s">
-        <v>892</v>
+        <v>888</v>
       </c>
       <c r="H323" s="24" t="s">
-        <v>893</v>
+        <v>889</v>
       </c>
       <c r="I323" s="24" t="s">
-        <v>891</v>
+        <v>887</v>
       </c>
       <c r="J323" s="25" t="s">
         <v>419</v>
@@ -18392,13 +18392,13 @@
         <v>419</v>
       </c>
       <c r="N323" s="25" t="s">
-        <v>888</v>
+        <v>884</v>
       </c>
       <c r="O323" s="25" t="s">
         <v>419</v>
       </c>
       <c r="P323" s="35" t="s">
-        <v>835</v>
+        <v>831</v>
       </c>
       <c r="Q323" s="25"/>
       <c r="R323" s="26"/>
@@ -18431,7 +18431,7 @@
         <v>422</v>
       </c>
       <c r="K324" s="25" t="s">
-        <v>894</v>
+        <v>890</v>
       </c>
       <c r="L324" s="35"/>
       <c r="M324" s="35"/>
@@ -18465,13 +18465,13 @@
         <v>45097</v>
       </c>
       <c r="G325" s="24" t="s">
-        <v>896</v>
+        <v>892</v>
       </c>
       <c r="H325" s="24" t="s">
-        <v>897</v>
+        <v>893</v>
       </c>
       <c r="I325" s="24" t="s">
-        <v>898</v>
+        <v>894</v>
       </c>
       <c r="J325" s="25" t="s">
         <v>419</v>
@@ -18484,13 +18484,13 @@
         <v>419</v>
       </c>
       <c r="N325" s="25" t="s">
-        <v>895</v>
+        <v>891</v>
       </c>
       <c r="O325" s="25" t="s">
         <v>419</v>
       </c>
       <c r="P325" s="35" t="s">
-        <v>835</v>
+        <v>831</v>
       </c>
       <c r="Q325" s="25"/>
       <c r="R325" s="26"/>
@@ -18519,13 +18519,13 @@
         <v>45097</v>
       </c>
       <c r="G326" s="24" t="s">
-        <v>900</v>
+        <v>896</v>
       </c>
       <c r="H326" s="24" t="s">
-        <v>901</v>
+        <v>897</v>
       </c>
       <c r="I326" s="24" t="s">
-        <v>902</v>
+        <v>898</v>
       </c>
       <c r="J326" s="25" t="s">
         <v>419</v>
@@ -18538,13 +18538,13 @@
         <v>419</v>
       </c>
       <c r="N326" s="25" t="s">
-        <v>899</v>
+        <v>895</v>
       </c>
       <c r="O326" s="25" t="s">
         <v>419</v>
       </c>
       <c r="P326" s="35" t="s">
-        <v>835</v>
+        <v>831</v>
       </c>
       <c r="Q326" s="25"/>
       <c r="R326" s="26"/>
@@ -18573,13 +18573,13 @@
         <v>45097</v>
       </c>
       <c r="G327" s="24" t="s">
-        <v>904</v>
+        <v>900</v>
       </c>
       <c r="H327" s="24" t="s">
-        <v>905</v>
+        <v>901</v>
       </c>
       <c r="I327" s="24" t="s">
-        <v>906</v>
+        <v>902</v>
       </c>
       <c r="J327" s="25" t="s">
         <v>419</v>
@@ -18592,13 +18592,13 @@
         <v>419</v>
       </c>
       <c r="N327" s="25" t="s">
-        <v>903</v>
+        <v>899</v>
       </c>
       <c r="O327" s="25" t="s">
         <v>419</v>
       </c>
       <c r="P327" s="35" t="s">
-        <v>835</v>
+        <v>831</v>
       </c>
       <c r="Q327" s="25"/>
       <c r="R327" s="26"/>
@@ -18631,7 +18631,7 @@
         <v>422</v>
       </c>
       <c r="K328" s="25" t="s">
-        <v>894</v>
+        <v>890</v>
       </c>
       <c r="L328" s="35"/>
       <c r="M328" s="35"/>
@@ -18669,7 +18669,7 @@
         <v>422</v>
       </c>
       <c r="K329" s="35" t="s">
-        <v>883</v>
+        <v>879</v>
       </c>
       <c r="L329" s="35"/>
       <c r="M329" s="35"/>

</xml_diff>